<commit_message>
updated references for falconidae, made correction of habitat to agriculture from grassland for Meyer
</commit_message>
<xml_diff>
--- a/cleaning/Meyer Avian Database.xlsx
+++ b/cleaning/Meyer Avian Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryu1\Documents\Ecological Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dietdatabase\cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t>Geomyidae</t>
-  </si>
-  <si>
-    <t>Grassland</t>
   </si>
   <si>
     <t>DR</t>
@@ -372,6 +369,9 @@
   </si>
   <si>
     <t>Male kestrel diet</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
   </si>
 </sst>
 </file>
@@ -1194,10 +1194,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Y1" sqref="Y1"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1365,7 @@
         <v>42</v>
       </c>
       <c r="M2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N2">
         <v>11</v>
@@ -1437,16 +1437,16 @@
         <v>1</v>
       </c>
       <c r="AK2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
@@ -1487,7 +1487,7 @@
         <v>42</v>
       </c>
       <c r="M3" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N3">
         <v>11</v>
@@ -1553,16 +1553,16 @@
         <v>1</v>
       </c>
       <c r="AK3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
@@ -1603,7 +1603,7 @@
         <v>42</v>
       </c>
       <c r="M4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N4">
         <v>11</v>
@@ -1675,16 +1675,16 @@
         <v>1</v>
       </c>
       <c r="AK4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
@@ -1725,7 +1725,7 @@
         <v>42</v>
       </c>
       <c r="M5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N5">
         <v>11</v>
@@ -1791,16 +1791,16 @@
         <v>1</v>
       </c>
       <c r="AK5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
@@ -1841,7 +1841,7 @@
         <v>42</v>
       </c>
       <c r="M6" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N6">
         <v>11</v>
@@ -1907,16 +1907,16 @@
         <v>1</v>
       </c>
       <c r="AK6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
@@ -1957,7 +1957,7 @@
         <v>42</v>
       </c>
       <c r="M7" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N7">
         <v>11</v>
@@ -2023,16 +2023,16 @@
         <v>1</v>
       </c>
       <c r="AK7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
@@ -2073,7 +2073,7 @@
         <v>42</v>
       </c>
       <c r="M8" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N8">
         <v>11</v>
@@ -2139,16 +2139,16 @@
         <v>1</v>
       </c>
       <c r="AK8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
@@ -2189,7 +2189,7 @@
         <v>42</v>
       </c>
       <c r="M9" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N9">
         <v>11</v>
@@ -2261,16 +2261,16 @@
         <v>1</v>
       </c>
       <c r="AK9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
@@ -2311,7 +2311,7 @@
         <v>42</v>
       </c>
       <c r="M10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N10">
         <v>11</v>
@@ -2380,16 +2380,16 @@
         <v>1</v>
       </c>
       <c r="AK10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
         <v>42</v>
       </c>
       <c r="M11" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N11">
         <v>11</v>
@@ -2502,16 +2502,16 @@
         <v>1</v>
       </c>
       <c r="AK11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
@@ -2552,7 +2552,7 @@
         <v>42</v>
       </c>
       <c r="M12" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N12">
         <v>11</v>
@@ -2624,16 +2624,16 @@
         <v>1</v>
       </c>
       <c r="AK12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
@@ -2674,7 +2674,7 @@
         <v>42</v>
       </c>
       <c r="M13" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N13">
         <v>11</v>
@@ -2743,16 +2743,16 @@
         <v>1</v>
       </c>
       <c r="AK13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN13" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
@@ -2793,7 +2793,7 @@
         <v>42</v>
       </c>
       <c r="M14" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N14">
         <v>11</v>
@@ -2865,16 +2865,16 @@
         <v>1</v>
       </c>
       <c r="AK14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
@@ -2915,7 +2915,7 @@
         <v>42</v>
       </c>
       <c r="M15" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N15">
         <v>11</v>
@@ -2987,16 +2987,16 @@
         <v>1</v>
       </c>
       <c r="AK15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
@@ -3037,7 +3037,7 @@
         <v>42</v>
       </c>
       <c r="M16" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N16">
         <v>11</v>
@@ -3109,16 +3109,16 @@
         <v>1</v>
       </c>
       <c r="AK16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
@@ -3159,7 +3159,7 @@
         <v>42</v>
       </c>
       <c r="M17" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N17">
         <v>11</v>
@@ -3231,16 +3231,16 @@
         <v>1</v>
       </c>
       <c r="AK17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
@@ -3281,7 +3281,7 @@
         <v>42</v>
       </c>
       <c r="M18" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N18">
         <v>11</v>
@@ -3350,16 +3350,16 @@
         <v>1</v>
       </c>
       <c r="AK18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
@@ -3400,7 +3400,7 @@
         <v>42</v>
       </c>
       <c r="M19" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N19">
         <v>11</v>
@@ -3472,16 +3472,16 @@
         <v>1</v>
       </c>
       <c r="AK19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
@@ -3522,7 +3522,7 @@
         <v>42</v>
       </c>
       <c r="M20" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N20">
         <v>11</v>
@@ -3594,16 +3594,16 @@
         <v>1</v>
       </c>
       <c r="AK20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
@@ -3644,7 +3644,7 @@
         <v>42</v>
       </c>
       <c r="M21" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N21">
         <v>11</v>
@@ -3716,16 +3716,16 @@
         <v>1</v>
       </c>
       <c r="AK21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
@@ -3766,7 +3766,7 @@
         <v>42</v>
       </c>
       <c r="M22" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N22">
         <v>11</v>
@@ -3838,16 +3838,16 @@
         <v>1</v>
       </c>
       <c r="AK22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
@@ -3888,7 +3888,7 @@
         <v>42</v>
       </c>
       <c r="M23" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N23">
         <v>11</v>
@@ -3960,16 +3960,16 @@
         <v>1</v>
       </c>
       <c r="AK23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN23" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
@@ -4010,7 +4010,7 @@
         <v>42</v>
       </c>
       <c r="M24" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N24">
         <v>11</v>
@@ -4082,16 +4082,16 @@
         <v>1</v>
       </c>
       <c r="AK24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN24" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
@@ -4132,7 +4132,7 @@
         <v>42</v>
       </c>
       <c r="M25" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N25">
         <v>11</v>
@@ -4204,16 +4204,16 @@
         <v>1</v>
       </c>
       <c r="AK25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
@@ -4254,7 +4254,7 @@
         <v>42</v>
       </c>
       <c r="M26" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N26">
         <v>11</v>
@@ -4326,16 +4326,16 @@
         <v>1</v>
       </c>
       <c r="AK26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN26" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
@@ -4376,7 +4376,7 @@
         <v>42</v>
       </c>
       <c r="M27" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N27">
         <v>11</v>
@@ -4448,16 +4448,16 @@
         <v>1</v>
       </c>
       <c r="AK27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN27" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
@@ -4498,7 +4498,7 @@
         <v>42</v>
       </c>
       <c r="M28" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N28">
         <v>11</v>
@@ -4558,7 +4558,7 @@
         <v>7.7681970000000004E-5</v>
       </c>
       <c r="AG28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH28">
         <v>740</v>
@@ -4570,16 +4570,16 @@
         <v>1</v>
       </c>
       <c r="AK28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN28" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.25">
@@ -4620,7 +4620,7 @@
         <v>42</v>
       </c>
       <c r="M29" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N29">
         <v>11</v>
@@ -4677,7 +4677,7 @@
         <v>2.99075585E-2</v>
       </c>
       <c r="AG29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH29">
         <v>740</v>
@@ -4689,16 +4689,16 @@
         <v>1</v>
       </c>
       <c r="AK29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN29" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
@@ -4739,7 +4739,7 @@
         <v>42</v>
       </c>
       <c r="M30" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N30">
         <v>11</v>
@@ -4799,7 +4799,7 @@
         <v>0.1050260235</v>
       </c>
       <c r="AG30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH30">
         <v>740</v>
@@ -4811,16 +4811,16 @@
         <v>1</v>
       </c>
       <c r="AK30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN30" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
@@ -4861,7 +4861,7 @@
         <v>42</v>
       </c>
       <c r="M31" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N31">
         <v>11</v>
@@ -4921,7 +4921,7 @@
         <v>2.2372407399999999E-2</v>
       </c>
       <c r="AG31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH31">
         <v>740</v>
@@ -4933,16 +4933,16 @@
         <v>1</v>
       </c>
       <c r="AK31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN31" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
@@ -4983,7 +4983,7 @@
         <v>42</v>
       </c>
       <c r="M32" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N32">
         <v>11</v>
@@ -5043,7 +5043,7 @@
         <v>1.4293482499999999E-2</v>
       </c>
       <c r="AG32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH32">
         <v>740</v>
@@ -5055,16 +5055,16 @@
         <v>1</v>
       </c>
       <c r="AK32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN32" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
@@ -5105,7 +5105,7 @@
         <v>42</v>
       </c>
       <c r="M33" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N33">
         <v>11</v>
@@ -5165,7 +5165,7 @@
         <v>6.742795E-2</v>
       </c>
       <c r="AG33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH33">
         <v>740</v>
@@ -5177,16 +5177,16 @@
         <v>1</v>
       </c>
       <c r="AK33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN33" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
@@ -5227,7 +5227,7 @@
         <v>42</v>
       </c>
       <c r="M34" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N34">
         <v>11</v>
@@ -5287,7 +5287,7 @@
         <v>3.93070768E-2</v>
       </c>
       <c r="AG34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH34">
         <v>740</v>
@@ -5299,16 +5299,16 @@
         <v>1</v>
       </c>
       <c r="AK34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN34" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.25">
@@ -5349,7 +5349,7 @@
         <v>42</v>
       </c>
       <c r="M35" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N35">
         <v>11</v>
@@ -5409,7 +5409,7 @@
         <v>0.2302493591</v>
       </c>
       <c r="AG35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH35">
         <v>740</v>
@@ -5421,16 +5421,16 @@
         <v>1</v>
       </c>
       <c r="AK35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN35" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
@@ -5471,7 +5471,7 @@
         <v>42</v>
       </c>
       <c r="M36" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N36">
         <v>11</v>
@@ -5531,7 +5531,7 @@
         <v>1.5536394E-2</v>
       </c>
       <c r="AG36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH36">
         <v>740</v>
@@ -5543,16 +5543,16 @@
         <v>1</v>
       </c>
       <c r="AK36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN36" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
@@ -5593,7 +5593,7 @@
         <v>42</v>
       </c>
       <c r="M37" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N37">
         <v>11</v>
@@ -5653,7 +5653,7 @@
         <v>2.3304591E-3</v>
       </c>
       <c r="AG37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH37">
         <v>740</v>
@@ -5665,16 +5665,16 @@
         <v>1</v>
       </c>
       <c r="AK37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN37" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
@@ -5715,7 +5715,7 @@
         <v>42</v>
       </c>
       <c r="M38" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N38">
         <v>11</v>
@@ -5775,7 +5775,7 @@
         <v>0.23281286409999999</v>
       </c>
       <c r="AG38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH38">
         <v>740</v>
@@ -5787,16 +5787,16 @@
         <v>1</v>
       </c>
       <c r="AK38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN38" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
@@ -5837,7 +5837,7 @@
         <v>42</v>
       </c>
       <c r="M39" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N39">
         <v>11</v>
@@ -5897,7 +5897,7 @@
         <v>9.3218364000000001E-3</v>
       </c>
       <c r="AG39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH39">
         <v>740</v>
@@ -5909,16 +5909,16 @@
         <v>1</v>
       </c>
       <c r="AK39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
@@ -5959,7 +5959,7 @@
         <v>42</v>
       </c>
       <c r="M40" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N40">
         <v>11</v>
@@ -6019,7 +6019,7 @@
         <v>5.8727569299999997E-2</v>
       </c>
       <c r="AG40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH40">
         <v>740</v>
@@ -6031,16 +6031,16 @@
         <v>1</v>
       </c>
       <c r="AK40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN40" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.25">
@@ -6081,7 +6081,7 @@
         <v>42</v>
       </c>
       <c r="M41" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N41">
         <v>11</v>
@@ -6141,7 +6141,7 @@
         <v>0.17260933740000001</v>
       </c>
       <c r="AG41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH41">
         <v>740</v>
@@ -6153,16 +6153,16 @@
         <v>1</v>
       </c>
       <c r="AK41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN41" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
@@ -6203,7 +6203,7 @@
         <v>42</v>
       </c>
       <c r="M42" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N42">
         <v>11</v>
@@ -6263,7 +6263,7 @@
         <v>1.5344484E-3</v>
       </c>
       <c r="AG42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH42">
         <v>755</v>
@@ -6275,16 +6275,16 @@
         <v>1</v>
       </c>
       <c r="AK42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN42" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
@@ -6325,7 +6325,7 @@
         <v>42</v>
       </c>
       <c r="M43" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N43">
         <v>11</v>
@@ -6385,7 +6385,7 @@
         <v>2.7620071E-3</v>
       </c>
       <c r="AG43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH43">
         <v>755</v>
@@ -6397,16 +6397,16 @@
         <v>1</v>
       </c>
       <c r="AK43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN43" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.25">
@@ -6447,7 +6447,7 @@
         <v>42</v>
       </c>
       <c r="M44" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N44">
         <v>11</v>
@@ -6501,7 +6501,7 @@
         <v>1.61117078E-2</v>
       </c>
       <c r="AG44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH44">
         <v>755</v>
@@ -6513,16 +6513,16 @@
         <v>1</v>
       </c>
       <c r="AK44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN44" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
@@ -6563,7 +6563,7 @@
         <v>42</v>
       </c>
       <c r="M45" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N45">
         <v>11</v>
@@ -6623,7 +6623,7 @@
         <v>0.22126745440000001</v>
       </c>
       <c r="AG45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH45">
         <v>755</v>
@@ -6635,16 +6635,16 @@
         <v>1</v>
       </c>
       <c r="AK45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN45" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:40" x14ac:dyDescent="0.25">
@@ -6685,7 +6685,7 @@
         <v>42</v>
       </c>
       <c r="M46" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N46">
         <v>11</v>
@@ -6745,7 +6745,7 @@
         <v>8.7310111999999995E-2</v>
       </c>
       <c r="AG46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH46">
         <v>755</v>
@@ -6757,16 +6757,16 @@
         <v>1</v>
       </c>
       <c r="AK46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN46" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:40" x14ac:dyDescent="0.25">
@@ -6807,7 +6807,7 @@
         <v>42</v>
       </c>
       <c r="M47" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N47">
         <v>11</v>
@@ -6867,7 +6867,7 @@
         <v>6.6595059100000006E-2</v>
       </c>
       <c r="AG47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH47">
         <v>755</v>
@@ -6879,16 +6879,16 @@
         <v>1</v>
       </c>
       <c r="AK47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN47" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.25">
@@ -6929,7 +6929,7 @@
         <v>42</v>
       </c>
       <c r="M48" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N48">
         <v>11</v>
@@ -6989,7 +6989,7 @@
         <v>0.19410771830000001</v>
       </c>
       <c r="AG48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH48">
         <v>755</v>
@@ -7001,16 +7001,16 @@
         <v>1</v>
       </c>
       <c r="AK48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:40" x14ac:dyDescent="0.25">
@@ -7051,7 +7051,7 @@
         <v>42</v>
       </c>
       <c r="M49" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N49">
         <v>11</v>
@@ -7111,7 +7111,7 @@
         <v>6.9970845500000003E-2</v>
       </c>
       <c r="AG49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH49">
         <v>755</v>
@@ -7123,16 +7123,16 @@
         <v>1</v>
       </c>
       <c r="AK49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN49" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.25">
@@ -7173,7 +7173,7 @@
         <v>42</v>
       </c>
       <c r="M50" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N50">
         <v>11</v>
@@ -7233,7 +7233,7 @@
         <v>1.9334049400000001E-2</v>
       </c>
       <c r="AG50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH50">
         <v>755</v>
@@ -7245,16 +7245,16 @@
         <v>1</v>
       </c>
       <c r="AK50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN50" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:40" x14ac:dyDescent="0.25">
@@ -7295,7 +7295,7 @@
         <v>42</v>
       </c>
       <c r="M51" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N51">
         <v>11</v>
@@ -7355,7 +7355,7 @@
         <v>0.11692496550000001</v>
       </c>
       <c r="AG51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH51">
         <v>755</v>
@@ -7367,16 +7367,16 @@
         <v>1</v>
       </c>
       <c r="AK51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN51" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:40" x14ac:dyDescent="0.25">
@@ -7417,7 +7417,7 @@
         <v>42</v>
       </c>
       <c r="M52" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N52">
         <v>11</v>
@@ -7477,7 +7477,7 @@
         <v>4.91023477E-2</v>
       </c>
       <c r="AG52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH52">
         <v>755</v>
@@ -7489,16 +7489,16 @@
         <v>1</v>
       </c>
       <c r="AK52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN52" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:40" x14ac:dyDescent="0.25">
@@ -7539,7 +7539,7 @@
         <v>42</v>
       </c>
       <c r="M53" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N53">
         <v>11</v>
@@ -7599,7 +7599,7 @@
         <v>0.15497928489999999</v>
       </c>
       <c r="AG53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH53">
         <v>755</v>
@@ -7611,16 +7611,16 @@
         <v>1</v>
       </c>
       <c r="AK53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AM53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN53" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>